<commit_message>
DMS: Translate AppUserStoreMapping Export and ExportTemplate
</commit_message>
<xml_diff>
--- a/DMS/Templates/AppUser_Store.xlsx
+++ b/DMS/Templates/AppUser_Store.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA46E84-3AE2-4456-BE4A-5DB214378B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DD1247-6841-4767-9CC5-4EB5958AFA36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AppUserStore" sheetId="1" r:id="rId1"/>
+    <sheet name="Phạm vi đi tuyến" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -59,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -434,7 +434,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
@@ -442,7 +442,7 @@
     <col min="4" max="4" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="25.5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -462,7 +462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -476,7 +476,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -488,7 +488,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>

</xml_diff>